<commit_message>
Bug-fix regarding the connection to the SQL-database
</commit_message>
<xml_diff>
--- a/master_time_sheet.xlsx
+++ b/master_time_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raghavakrishna\OneDrive - bwedu\5_PythonFiles\ESHL_CBo_Post_Processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sauerswa\wichtige Ordner\sauerswa\Codes\Python\ESHL_CBo_Post_Processing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCA17DA-543D-4823-8112-D0C54D96C934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4AA69E-787C-4B07-9DA8-BE35B7869026}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="16080" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,19 @@
     <sheet name="wall_CBO" sheetId="6" r:id="rId8"/>
     <sheet name="wall_ESHL" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -46,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -55,7 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 These names should be given as input for analysis. Alternatively you could create a simple GUI to select this column.</t>
@@ -70,7 +79,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -79,7 +88,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 These seonsors are excluded from evaluation</t>
@@ -94,7 +103,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -103,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 The database to look for calibration regression equations.</t>
@@ -118,7 +127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -127,7 +136,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 No outdoor CO2 data</t>
@@ -142,7 +151,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -151,7 +160,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 No outdoor CO2 data
@@ -177,7 +186,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -186,7 +195,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 All the inputs are previously calculated using python and the corresponding results with its uncertainties are listed here to reduce computing power.
@@ -213,7 +222,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -222,7 +231,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 SZ 01 CBO winter</t>
@@ -237,7 +246,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -246,7 +255,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 SZ 02 CBO winter</t>
@@ -261,7 +270,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -270,7 +279,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 WZ CBO winter</t>
@@ -285,7 +294,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -294,7 +303,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 BD winter</t>
@@ -319,7 +328,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -328,7 +337,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 SZ 01 CBO winter</t>
@@ -343,7 +352,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -352,7 +361,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 SZ 02 CBO winter</t>
@@ -367,7 +376,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -376,7 +385,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 WZ CBO winter</t>
@@ -391,7 +400,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -400,7 +409,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 BD winter</t>
@@ -425,7 +434,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -434,7 +443,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Winter measurements</t>
@@ -449,7 +458,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -458,7 +467,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Summer measurements</t>
@@ -483,7 +492,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -492,7 +501,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 ESHL Winter naming conventions</t>
@@ -507,7 +516,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -516,7 +525,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 ESHL Summer naming conventions</t>
@@ -541,7 +550,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -550,7 +559,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 This sheet has the names of columns and the standardised columns. This way it is easy to identlfy the sensor and units just by seeing column name in MySQL database. </t>
@@ -565,7 +574,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -574,7 +583,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Winter</t>
@@ -589,7 +598,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -598,7 +607,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Summer</t>
@@ -613,7 +622,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -622,7 +631,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Testo 350XL</t>
@@ -637,7 +646,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -646,7 +655,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Testo 350XL</t>
@@ -661,7 +670,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -670,7 +679,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Testo 480</t>
@@ -685,7 +694,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -694,7 +703,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Testo 400</t>
@@ -719,7 +728,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -728,7 +737,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Winter measurements</t>
@@ -743,7 +752,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -752,7 +761,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Summer measurements</t>
@@ -777,7 +786,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -786,7 +795,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Summer measurements</t>
@@ -801,7 +810,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Raghavakrishna Devineni:</t>
         </r>
@@ -810,7 +819,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Winter measurements</t>
@@ -1811,14 +1820,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2295,8 +2304,8 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Eingabe" xfId="1" builtinId="20"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2577,19 +2586,19 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.1796875" customWidth="1"/>
-    <col min="2" max="3" width="18.54296875" customWidth="1"/>
-    <col min="4" max="4" width="22.7265625" customWidth="1"/>
+    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="2" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="68" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2612,7 +2621,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2635,7 +2644,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2658,7 +2667,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2681,7 +2690,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -2704,7 +2713,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -2727,7 +2736,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2750,7 +2759,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -2773,7 +2782,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -2796,7 +2805,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -2819,7 +2828,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -2842,7 +2851,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -2865,7 +2874,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2888,7 +2897,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>15</v>
       </c>
@@ -2911,7 +2920,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>16</v>
       </c>
@@ -2934,7 +2943,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
@@ -2957,7 +2966,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -2980,7 +2989,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>19</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>21</v>
       </c>
@@ -3049,7 +3058,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -3087,21 +3096,21 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -3133,7 +3142,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
@@ -3165,7 +3174,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>16</v>
       </c>
@@ -3197,7 +3206,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>17</v>
       </c>
@@ -3229,7 +3238,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>18</v>
       </c>
@@ -3261,7 +3270,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>19</v>
       </c>
@@ -3293,7 +3302,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
@@ -3325,7 +3334,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>21</v>
       </c>
@@ -3357,7 +3366,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>22</v>
       </c>
@@ -3389,7 +3398,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
@@ -3421,7 +3430,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>4</v>
       </c>
@@ -3453,7 +3462,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>5</v>
       </c>
@@ -3485,7 +3494,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>6</v>
       </c>
@@ -3517,7 +3526,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>7</v>
       </c>
@@ -3549,7 +3558,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>8</v>
       </c>
@@ -3581,7 +3590,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>9</v>
       </c>
@@ -3613,7 +3622,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>10</v>
       </c>
@@ -3645,7 +3654,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>11</v>
       </c>
@@ -3677,7 +3686,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>12</v>
       </c>
@@ -3709,7 +3718,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>13</v>
       </c>
@@ -3741,7 +3750,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>14</v>
       </c>
@@ -3788,19 +3797,19 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.90625" customWidth="1"/>
-    <col min="8" max="8" width="20.7265625" customWidth="1"/>
-    <col min="10" max="10" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
         <v>79</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="63" t="s">
         <v>81</v>
       </c>
@@ -3852,7 +3861,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="63" t="s">
         <v>83</v>
       </c>
@@ -3878,7 +3887,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">
         <v>85</v>
       </c>
@@ -3904,7 +3913,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="63" t="s">
         <v>164</v>
       </c>
@@ -3930,7 +3939,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
         <v>165</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="63" t="s">
         <v>101</v>
       </c>
@@ -3982,7 +3991,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="63" t="s">
         <v>166</v>
       </c>
@@ -4008,7 +4017,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="63" t="s">
         <v>167</v>
       </c>
@@ -4034,7 +4043,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="63" t="s">
         <v>104</v>
       </c>
@@ -4054,7 +4063,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
         <v>168</v>
       </c>
@@ -4074,7 +4083,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>106</v>
       </c>
@@ -4106,9 +4115,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="81" t="s">
         <v>79</v>
       </c>
@@ -4137,7 +4146,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="75" t="s">
         <v>109</v>
       </c>
@@ -4163,7 +4172,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="75" t="s">
         <v>179</v>
       </c>
@@ -4189,7 +4198,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="75" t="s">
         <v>85</v>
       </c>
@@ -4215,7 +4224,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="75" t="s">
         <v>180</v>
       </c>
@@ -4241,7 +4250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="75" t="s">
         <v>181</v>
       </c>
@@ -4267,7 +4276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="75" t="s">
         <v>182</v>
       </c>
@@ -4293,7 +4302,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="75" t="s">
         <v>173</v>
       </c>
@@ -4319,7 +4328,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="75" t="s">
         <v>174</v>
       </c>
@@ -4345,7 +4354,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="75" t="s">
         <v>183</v>
       </c>
@@ -4365,7 +4374,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="75" t="s">
         <v>99</v>
       </c>
@@ -4385,7 +4394,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
         <v>101</v>
       </c>
@@ -4405,7 +4414,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G13" s="79" t="s">
         <v>195</v>
       </c>
@@ -4413,7 +4422,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G14" s="77" t="s">
         <v>110</v>
       </c>
@@ -4421,7 +4430,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G15" s="77" t="s">
         <v>111</v>
       </c>
@@ -4429,7 +4438,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G16" s="77" t="s">
         <v>112</v>
       </c>
@@ -4437,7 +4446,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G17" s="77" t="s">
         <v>113</v>
       </c>
@@ -4445,7 +4454,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G18" s="77" t="s">
         <v>115</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G19" s="77" t="s">
         <v>117</v>
       </c>
@@ -4461,7 +4470,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G20" s="77" t="s">
         <v>118</v>
       </c>
@@ -4469,7 +4478,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G21" s="77" t="s">
         <v>119</v>
       </c>
@@ -4477,7 +4486,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G22" s="77" t="s">
         <v>175</v>
       </c>
@@ -4485,7 +4494,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G23" s="77" t="s">
         <v>176</v>
       </c>
@@ -4493,7 +4502,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G24" s="77" t="s">
         <v>196</v>
       </c>
@@ -4515,9 +4524,9 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>47</v>
       </c>
@@ -4531,7 +4540,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>129</v>
       </c>
@@ -4545,7 +4554,7 @@
         <v>20274900</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="54" t="s">
         <v>50</v>
       </c>
@@ -4559,7 +4568,7 @@
         <v>20269839</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="54" t="s">
         <v>52</v>
       </c>
@@ -4573,7 +4582,7 @@
         <v>20274901</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="53" t="s">
         <v>53</v>
       </c>
@@ -4587,7 +4596,7 @@
         <v>10773515</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
         <v>54</v>
       </c>
@@ -4601,7 +4610,7 @@
         <v>20269806</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
         <v>130</v>
       </c>
@@ -4615,7 +4624,7 @@
         <v>10950495</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
         <v>55</v>
       </c>
@@ -4629,7 +4638,7 @@
         <v>10950492</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>56</v>
       </c>
@@ -4643,7 +4652,7 @@
         <v>20269834</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>58</v>
       </c>
@@ -4657,7 +4666,7 @@
         <v>10773514</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>59</v>
       </c>
@@ -4671,7 +4680,7 @@
         <v>20269811</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="53" t="s">
         <v>61</v>
       </c>
@@ -4685,7 +4694,7 @@
         <v>20269842</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="54" t="s">
         <v>62</v>
       </c>
@@ -4699,7 +4708,7 @@
         <v>20269828</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
         <v>63</v>
       </c>
@@ -4713,7 +4722,7 @@
         <v>10950491</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
         <v>64</v>
       </c>
@@ -4727,7 +4736,7 @@
         <v>10950493</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
         <v>66</v>
       </c>
@@ -4741,7 +4750,7 @@
         <v>20269831</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
         <v>67</v>
       </c>
@@ -4755,7 +4764,7 @@
         <v>20269838</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="53" t="s">
         <v>69</v>
       </c>
@@ -4769,7 +4778,7 @@
         <v>20269833</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
         <v>70</v>
       </c>
@@ -4783,7 +4792,7 @@
         <v>20269827</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="53" t="s">
         <v>71</v>
       </c>
@@ -4797,7 +4806,7 @@
         <v>10773512</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="53" t="s">
         <v>131</v>
       </c>
@@ -4811,7 +4820,7 @@
         <v>20269840</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="53" t="s">
         <v>132</v>
       </c>
@@ -4825,7 +4834,7 @@
         <v>20269829</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="53" t="s">
         <v>133</v>
       </c>
@@ -4839,7 +4848,7 @@
         <v>20269841</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>134</v>
       </c>
@@ -4853,7 +4862,7 @@
         <v>20269832</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="54" t="s">
         <v>76</v>
       </c>
@@ -4867,7 +4876,7 @@
         <v>20269835</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="55" t="s">
         <v>77</v>
       </c>
@@ -4875,7 +4884,7 @@
         <v>20269832</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="55" t="s">
         <v>135</v>
       </c>
@@ -4883,7 +4892,7 @@
         <v>10773513</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="s">
         <v>136</v>
       </c>
@@ -4891,7 +4900,7 @@
         <v>20274900</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
         <v>78</v>
       </c>
@@ -4899,7 +4908,7 @@
         <v>20269835</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="54" t="s">
         <v>137</v>
       </c>
@@ -4907,7 +4916,7 @@
         <v>20269836</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="54" t="s">
         <v>138</v>
       </c>
@@ -4915,7 +4924,7 @@
         <v>10950494</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="54" t="s">
         <v>139</v>
       </c>
@@ -4937,9 +4946,9 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>47</v>
       </c>
@@ -4953,7 +4962,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
         <v>49</v>
       </c>
@@ -4967,7 +4976,7 @@
         <v>20269827</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>50</v>
       </c>
@@ -4981,7 +4990,7 @@
         <v>20269829</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>51</v>
       </c>
@@ -4995,7 +5004,7 @@
         <v>10773513</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
         <v>52</v>
       </c>
@@ -5009,7 +5018,7 @@
         <v>20269838</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>53</v>
       </c>
@@ -5023,7 +5032,7 @@
         <v>20269832</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
         <v>54</v>
       </c>
@@ -5037,7 +5046,7 @@
         <v>20269833</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>55</v>
       </c>
@@ -5051,7 +5060,7 @@
         <v>20269834</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>56</v>
       </c>
@@ -5065,7 +5074,7 @@
         <v>10773515</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>57</v>
       </c>
@@ -5079,7 +5088,7 @@
         <v>20269839</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>58</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>10773512</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="34" t="s">
         <v>59</v>
       </c>
@@ -5107,7 +5116,7 @@
         <v>20269837</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>60</v>
       </c>
@@ -5121,7 +5130,7 @@
         <v>20269830</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
         <v>61</v>
       </c>
@@ -5135,7 +5144,7 @@
         <v>20269840</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>62</v>
       </c>
@@ -5149,7 +5158,7 @@
         <v>20269836</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>63</v>
       </c>
@@ -5163,7 +5172,7 @@
         <v>10950491</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
         <v>64</v>
       </c>
@@ -5177,7 +5186,7 @@
         <v>20269835</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="34" t="s">
         <v>65</v>
       </c>
@@ -5191,7 +5200,7 @@
         <v>10773511</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="36" t="s">
         <v>66</v>
       </c>
@@ -5205,7 +5214,7 @@
         <v>20269841</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
         <v>67</v>
       </c>
@@ -5219,7 +5228,7 @@
         <v>20269806</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>68</v>
       </c>
@@ -5233,7 +5242,7 @@
         <v>10950493</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
         <v>69</v>
       </c>
@@ -5247,7 +5256,7 @@
         <v>20274900</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>70</v>
       </c>
@@ -5261,7 +5270,7 @@
         <v>10950494</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="34" t="s">
         <v>71</v>
       </c>
@@ -5275,7 +5284,7 @@
         <v>20269831</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="36" t="s">
         <v>72</v>
       </c>
@@ -5289,7 +5298,7 @@
         <v>20269811</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="34" t="s">
         <v>73</v>
       </c>
@@ -5303,7 +5312,7 @@
         <v>10950492</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="38" t="s">
         <v>74</v>
       </c>
@@ -5317,7 +5326,7 @@
         <v>10950495</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="34" t="s">
         <v>75</v>
       </c>
@@ -5331,7 +5340,7 @@
         <v>10773514</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="36" t="s">
         <v>76</v>
       </c>
@@ -5345,7 +5354,7 @@
         <v>20269842</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>77</v>
       </c>
@@ -5359,7 +5368,7 @@
         <v>20274901</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="38" t="s">
         <v>78</v>
       </c>
@@ -5387,15 +5396,15 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>79</v>
       </c>
@@ -5422,7 +5431,7 @@
       <c r="P1" s="41"/>
       <c r="Q1" s="41"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="49" t="s">
         <v>81</v>
       </c>
@@ -5449,7 +5458,7 @@
       <c r="P2" s="41"/>
       <c r="Q2" s="41"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>83</v>
       </c>
@@ -5476,7 +5485,7 @@
       <c r="P3" s="44"/>
       <c r="Q3" s="44"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>85</v>
       </c>
@@ -5503,7 +5512,7 @@
       <c r="P4" s="47"/>
       <c r="Q4" s="47"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
         <v>87</v>
       </c>
@@ -5530,7 +5539,7 @@
       <c r="P5" s="48"/>
       <c r="Q5" s="47"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>89</v>
       </c>
@@ -5557,7 +5566,7 @@
       <c r="P6" s="48"/>
       <c r="Q6" s="47"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
         <v>91</v>
       </c>
@@ -5584,7 +5593,7 @@
       <c r="P7" s="48"/>
       <c r="Q7" s="47"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
         <v>93</v>
       </c>
@@ -5611,7 +5620,7 @@
       <c r="P8" s="48"/>
       <c r="Q8" s="47"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>95</v>
       </c>
@@ -5638,7 +5647,7 @@
       <c r="P9" s="44"/>
       <c r="Q9" s="44"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
         <v>97</v>
       </c>
@@ -5665,7 +5674,7 @@
       <c r="P10" s="41"/>
       <c r="Q10" s="41"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
         <v>99</v>
       </c>
@@ -5692,7 +5701,7 @@
       <c r="P11" s="41"/>
       <c r="Q11" s="41"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
         <v>101</v>
       </c>
@@ -5719,7 +5728,7 @@
       <c r="P12" s="41"/>
       <c r="Q12" s="41"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
         <v>81</v>
       </c>
@@ -5746,7 +5755,7 @@
       <c r="P13" s="41"/>
       <c r="Q13" s="41"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="49" t="s">
         <v>83</v>
       </c>
@@ -5773,7 +5782,7 @@
       <c r="P14" s="41"/>
       <c r="Q14" s="41"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
         <v>85</v>
       </c>
@@ -5800,7 +5809,7 @@
       <c r="P15" s="41"/>
       <c r="Q15" s="41"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="49" t="s">
         <v>103</v>
       </c>
@@ -5827,7 +5836,7 @@
       <c r="P16" s="41"/>
       <c r="Q16" s="41"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="49" t="s">
         <v>99</v>
       </c>
@@ -5841,7 +5850,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="49" t="s">
         <v>101</v>
       </c>
@@ -5855,7 +5864,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
         <v>104</v>
       </c>
@@ -5869,7 +5878,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="49" t="s">
         <v>105</v>
       </c>
@@ -5883,7 +5892,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
         <v>106</v>
       </c>
@@ -5897,7 +5906,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="49" t="s">
         <v>107</v>
       </c>
@@ -5911,7 +5920,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>108</v>
       </c>
@@ -5925,7 +5934,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="43" t="s">
         <v>109</v>
       </c>
@@ -5939,7 +5948,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
         <v>110</v>
       </c>
@@ -5953,7 +5962,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
         <v>111</v>
       </c>
@@ -5967,7 +5976,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="50" t="s">
         <v>112</v>
       </c>
@@ -5981,7 +5990,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
         <v>113</v>
       </c>
@@ -5995,7 +6004,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>115</v>
       </c>
@@ -6009,7 +6018,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
         <v>117</v>
       </c>
@@ -6023,7 +6032,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
         <v>118</v>
       </c>
@@ -6037,7 +6046,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>119</v>
       </c>
@@ -6051,7 +6060,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="43" t="s">
         <v>120</v>
       </c>
@@ -6065,7 +6074,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="41" t="s">
         <v>122</v>
       </c>
@@ -6079,7 +6088,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
         <v>124</v>
       </c>
@@ -6093,7 +6102,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="41" t="s">
         <v>126</v>
       </c>
@@ -6107,7 +6116,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="41" t="s">
         <v>127</v>
       </c>
@@ -6121,7 +6130,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
         <v>128</v>
       </c>
@@ -6149,9 +6158,9 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>47</v>
       </c>
@@ -6165,7 +6174,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>140</v>
       </c>
@@ -6179,7 +6188,7 @@
         <v>9759956</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>141</v>
       </c>
@@ -6193,7 +6202,7 @@
         <v>10811406</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>142</v>
       </c>
@@ -6207,7 +6216,7 @@
         <v>1222778</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>143</v>
       </c>
@@ -6221,7 +6230,7 @@
         <v>9759954</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>144</v>
       </c>
@@ -6235,7 +6244,7 @@
         <v>1222769</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>145</v>
       </c>
@@ -6249,7 +6258,7 @@
         <v>10811400</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>146</v>
       </c>
@@ -6263,7 +6272,7 @@
         <v>10811408</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>147</v>
       </c>
@@ -6277,7 +6286,7 @@
         <v>1222777</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>148</v>
       </c>
@@ -6291,7 +6300,7 @@
         <v>9759955</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>149</v>
       </c>
@@ -6305,7 +6314,7 @@
         <v>1222771</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="58" t="s">
         <v>150</v>
       </c>
@@ -6319,7 +6328,7 @@
         <v>1222772</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
         <v>151</v>
       </c>
@@ -6333,7 +6342,7 @@
         <v>1222767</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>152</v>
       </c>
@@ -6347,7 +6356,7 @@
         <v>10811409</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
         <v>153</v>
       </c>
@@ -6361,7 +6370,7 @@
         <v>10811411</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="58" t="s">
         <v>154</v>
       </c>
@@ -6375,7 +6384,7 @@
         <v>10811401</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
         <v>155</v>
       </c>
@@ -6389,7 +6398,7 @@
         <v>1222768</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="58" t="s">
         <v>156</v>
       </c>
@@ -6403,7 +6412,7 @@
         <v>1222770</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="58" t="s">
         <v>157</v>
       </c>
@@ -6417,7 +6426,7 @@
         <v>1222776</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
         <v>158</v>
       </c>
@@ -6431,7 +6440,7 @@
         <v>1222765</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="58" t="s">
         <v>159</v>
       </c>
@@ -6445,7 +6454,7 @@
         <v>1222775</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="58" t="s">
         <v>160</v>
       </c>
@@ -6459,7 +6468,7 @@
         <v>10811404</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="58" t="s">
         <v>161</v>
       </c>
@@ -6473,7 +6482,7 @@
         <v>9759958</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="58" t="s">
         <v>162</v>
       </c>
@@ -6487,7 +6496,7 @@
         <v>10811399</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="58" t="s">
         <v>163</v>
       </c>
@@ -6515,12 +6524,12 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="93" t="s">
         <v>235</v>
       </c>
@@ -6540,7 +6549,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="92" t="s">
         <v>140</v>
       </c>
@@ -6560,7 +6569,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
         <v>141</v>
       </c>
@@ -6580,7 +6589,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="92" t="s">
         <v>142</v>
       </c>
@@ -6600,7 +6609,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="92" t="s">
         <v>143</v>
       </c>
@@ -6620,7 +6629,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
         <v>144</v>
       </c>
@@ -6640,7 +6649,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
         <v>145</v>
       </c>
@@ -6660,7 +6669,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
         <v>146</v>
       </c>
@@ -6680,7 +6689,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="92" t="s">
         <v>147</v>
       </c>
@@ -6700,7 +6709,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="92" t="s">
         <v>148</v>
       </c>
@@ -6720,7 +6729,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="92" t="s">
         <v>149</v>
       </c>
@@ -6740,7 +6749,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="92" t="s">
         <v>150</v>
       </c>
@@ -6760,7 +6769,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="92" t="s">
         <v>151</v>
       </c>
@@ -6780,7 +6789,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="92" t="s">
         <v>152</v>
       </c>
@@ -6800,7 +6809,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="92" t="s">
         <v>153</v>
       </c>
@@ -6811,7 +6820,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="92" t="s">
         <v>154</v>
       </c>
@@ -6822,7 +6831,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="92" t="s">
         <v>155</v>
       </c>
@@ -6833,7 +6842,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
         <v>156</v>
       </c>
@@ -6844,7 +6853,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
         <v>157</v>
       </c>
@@ -6855,7 +6864,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="92" t="s">
         <v>158</v>
       </c>
@@ -6866,7 +6875,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="92" t="s">
         <v>159</v>
       </c>
@@ -6877,7 +6886,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="92" t="s">
         <v>160</v>
       </c>
@@ -6888,7 +6897,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="92" t="s">
         <v>161</v>
       </c>
@@ -6899,7 +6908,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="92" t="s">
         <v>162</v>
       </c>
@@ -6910,7 +6919,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="92" t="s">
         <v>163</v>
       </c>
@@ -6921,7 +6930,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="92" t="s">
         <v>286</v>
       </c>
@@ -6932,7 +6941,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="92" t="s">
         <v>289</v>
       </c>
@@ -6943,7 +6952,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="92" t="s">
         <v>292</v>
       </c>
@@ -6954,7 +6963,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="92" t="s">
         <v>295</v>
       </c>
@@ -6965,7 +6974,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="92" t="s">
         <v>298</v>
       </c>
@@ -6976,7 +6985,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="92" t="s">
         <v>301</v>
       </c>

</xml_diff>